<commit_message>
editted report v2 again
</commit_message>
<xml_diff>
--- a/report/graphs/graphs_main.xlsx
+++ b/report/graphs/graphs_main.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>n</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>Weak Scaling</t>
   </si>
   <si>
     <t>Strong Scaling</t>
@@ -2453,6 +2456,566 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>OpenMP: Weak Scaling</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0955065698752022"/>
+          <c:y val="0.0787541688505389"/>
+          <c:w val="0.866917939078277"/>
+          <c:h val="0.831349725869639"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>4000 particles per thread</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.205152348822013"/>
+                  <c:y val="0.128402905520158"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$3:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$3:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.651965</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.837759</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.077</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.29095</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.55135</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.53885</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2090212048"/>
+        <c:axId val="-2097038656"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2090212048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="25.0"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2097038656"/>
+        <c:crossesAt val="0.01"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1.0"/>
+        <c:minorUnit val="0.5"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2097038656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5.0"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2090212048"/>
+        <c:crossesAt val="0.0"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.572123853352515"/>
+          <c:y val="0.101955054078525"/>
+          <c:w val="0.204356573364406"/>
+          <c:h val="0.152600889892105"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2573,6 +3136,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3606,6 +4209,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4188,15 +5307,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>660598</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>681764</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>116417</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>494673</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>515839</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4212,6 +5331,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>380999</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>10583</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>215074</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>84666</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4485,17 +5636,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.2">
       <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
@@ -4529,7 +5685,7 @@
         <v>6</v>
       </c>
       <c r="L2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
@@ -4642,7 +5798,7 @@
         <v>3.4854999999999997E-2</v>
       </c>
       <c r="J6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K6">
         <v>1.29095</v>
@@ -4671,7 +5827,7 @@
         <v>4.5162000000000001E-2</v>
       </c>
       <c r="J7">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="K7">
         <v>2.5513499999999998</v>
@@ -4703,10 +5859,10 @@
         <v>24</v>
       </c>
       <c r="K8">
-        <v>4.1139400000000004</v>
+        <v>2.5388500000000001</v>
       </c>
       <c r="L8">
-        <v>128000</v>
+        <v>96000</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
@@ -4722,6 +5878,9 @@
       <c r="E9">
         <v>0.44569900000000001</v>
       </c>
+      <c r="G9">
+        <v>2000</v>
+      </c>
       <c r="H9">
         <v>1</v>
       </c>
@@ -4739,9 +5898,6 @@
       <c r="E10">
         <v>0.88995100000000005</v>
       </c>
-      <c r="G10">
-        <v>2000</v>
-      </c>
       <c r="H10">
         <v>2</v>
       </c>
@@ -4809,6 +5965,9 @@
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <v>8000</v>
+      </c>
       <c r="H15">
         <v>1</v>
       </c>
@@ -4825,9 +5984,6 @@
       </c>
     </row>
     <row r="17" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G17">
-        <v>8000</v>
-      </c>
       <c r="H17">
         <v>4</v>
       </c>
@@ -4860,6 +6016,9 @@
       </c>
     </row>
     <row r="21" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <v>32000</v>
+      </c>
       <c r="H21">
         <v>1</v>
       </c>
@@ -4884,9 +6043,6 @@
       </c>
     </row>
     <row r="24" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G24">
-        <v>32000</v>
-      </c>
       <c r="H24">
         <v>6</v>
       </c>
@@ -4911,6 +6067,9 @@
       </c>
     </row>
     <row r="27" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <v>128000</v>
+      </c>
       <c r="H27">
         <v>1</v>
       </c>
@@ -4943,9 +6102,6 @@
       </c>
     </row>
     <row r="31" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G31">
-        <v>128000</v>
-      </c>
       <c r="H31">
         <v>12</v>
       </c>
@@ -4962,8 +6118,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>